<commit_message>
[PLANNING] Started first pass on planning master document
</commit_message>
<xml_diff>
--- a/Development/Planning/TaskPlanning.xlsx
+++ b/Development/Planning/TaskPlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Dawn of War Soulstorm\TFE\Development\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F223887F-E50C-43DD-8517-818CC1415BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CEBE5A-B14F-4FA9-8107-E3C278C1A58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,10 @@
     <sheet name="Code" sheetId="8" r:id="rId2"/>
     <sheet name="Audio" sheetId="10" r:id="rId3"/>
     <sheet name="Art" sheetId="1" r:id="rId4"/>
-    <sheet name="QA" sheetId="12" r:id="rId5"/>
-    <sheet name="Production" sheetId="13" r:id="rId6"/>
-    <sheet name="Macro" sheetId="7" r:id="rId7"/>
+    <sheet name="Maps" sheetId="14" r:id="rId5"/>
+    <sheet name="QA" sheetId="12" r:id="rId6"/>
+    <sheet name="Production" sheetId="13" r:id="rId7"/>
+    <sheet name="Macro" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="149">
   <si>
     <t>Task</t>
   </si>
@@ -141,6 +142,354 @@
   </si>
   <si>
     <t>Ready For Approval</t>
+  </si>
+  <si>
+    <t>Ard Boy - EBPs, SBPs, Weapons</t>
+  </si>
+  <si>
+    <t>Skar Boy - EBPs, SBPs, Weapons</t>
+  </si>
+  <si>
+    <t>Feral Boy Possession Global Ability</t>
+  </si>
+  <si>
+    <t>Ard Boy attach ranged weapon swapping</t>
+  </si>
+  <si>
+    <t>Tyranid Scout Unit Design</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>We need to decide on a design for this unit then write up that design</t>
+  </si>
+  <si>
+    <t>Balancing Tau</t>
+  </si>
+  <si>
+    <t>Finish initial rosta for Tyranids</t>
+  </si>
+  <si>
+    <t>Tau upkeep</t>
+  </si>
+  <si>
+    <t>Sisters Faith Rework</t>
+  </si>
+  <si>
+    <t>Armour Resistance Rework</t>
+  </si>
+  <si>
+    <t>This is blocking any upkeep</t>
+  </si>
+  <si>
+    <t>Implementing armour modifier to more places</t>
+  </si>
+  <si>
+    <t>Mass / Knockback Rework</t>
+  </si>
+  <si>
+    <t>OM add in leman variant unit</t>
+  </si>
+  <si>
+    <t>OM Assault Chim T3 weapon upgrade to assault cannon</t>
+  </si>
+  <si>
+    <t>OM Leman Russ alt model from unification mod</t>
+  </si>
+  <si>
+    <t>OM Assault Chimera model from unification mod</t>
+  </si>
+  <si>
+    <t>OM Check current assualt chimera to see if it supports autocannon</t>
+  </si>
+  <si>
+    <t>Revisit current global abilities design</t>
+  </si>
+  <si>
+    <t>Design for Tyranids global abilities</t>
+  </si>
+  <si>
+    <t>Design for OM global abilities</t>
+  </si>
+  <si>
+    <t>Design for Tau global abilities</t>
+  </si>
+  <si>
+    <t>Decide how upkeep works in early game</t>
+  </si>
+  <si>
+    <t>Do we want people to have a certain number of points / gens before we charge them?</t>
+  </si>
+  <si>
+    <t>Setup ability target filters for new armours</t>
+  </si>
+  <si>
+    <t>Add piercings to abilities</t>
+  </si>
+  <si>
+    <t>Decide which maps we wish to create TFE variants for</t>
+  </si>
+  <si>
+    <t>Air unit fix for MoM TFE</t>
+  </si>
+  <si>
+    <t>Air unit fix for SoE TFE</t>
+  </si>
+  <si>
+    <t>Air unit fix for TE TFE</t>
+  </si>
+  <si>
+    <t>Decide what we're doing with Sarajevo map</t>
+  </si>
+  <si>
+    <t>I think this is already done..?</t>
+  </si>
+  <si>
+    <t>TFE Variant of BM</t>
+  </si>
+  <si>
+    <t>TFE Variant of FM</t>
+  </si>
+  <si>
+    <t>TFE Variant of BR</t>
+  </si>
+  <si>
+    <t>TFE Variant of EG</t>
+  </si>
+  <si>
+    <t>TFE Variant of FC</t>
+  </si>
+  <si>
+    <t>TFE Variant of MoM</t>
+  </si>
+  <si>
+    <t>TFE Variant of SoE</t>
+  </si>
+  <si>
+    <t>Air unit fix for FM TFE</t>
+  </si>
+  <si>
+    <t>Air unit fix for BM TFE</t>
+  </si>
+  <si>
+    <t>Air unit fix for BR TFE</t>
+  </si>
+  <si>
+    <t>Air unit fix for EG TFE</t>
+  </si>
+  <si>
+    <t>Air unit fix for FC TFE</t>
+  </si>
+  <si>
+    <t>TFE Variant of TE</t>
+  </si>
+  <si>
+    <t>Decide what new maps to make</t>
+  </si>
+  <si>
+    <t>Widen pathing, fix stair collision, make impassable terrain clearer</t>
+  </si>
+  <si>
+    <t>Revisit BRV Design</t>
+  </si>
+  <si>
+    <t>BRV Faction</t>
+  </si>
+  <si>
+    <t>New (and multiplayer?) Campaign</t>
+  </si>
+  <si>
+    <t>Tutorial/Demo level</t>
+  </si>
+  <si>
+    <t>Revisit design for Alpha Legion subfaction</t>
+  </si>
+  <si>
+    <t>Model for Champs Of Tzeentch</t>
+  </si>
+  <si>
+    <t>Model for Noise Marines</t>
+  </si>
+  <si>
+    <t>Model for Stalk Defiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chaos Preds Variants Possession </t>
+  </si>
+  <si>
+    <t>Remove predator variants from machine pit</t>
+  </si>
+  <si>
+    <t>Obliterator abilities effects</t>
+  </si>
+  <si>
+    <t>Stalk defiler frenzy ability effects</t>
+  </si>
+  <si>
+    <t>Chaos scout unit effect</t>
+  </si>
+  <si>
+    <t>Simple model for scout unit trap</t>
+  </si>
+  <si>
+    <t>Use a single mine from the mine fiels</t>
+  </si>
+  <si>
+    <t>Check if khorne zerks require more iteration</t>
+  </si>
+  <si>
+    <t>Edit khorne zerks model so they get 2 axes in T3</t>
+  </si>
+  <si>
+    <t>Cultist worship audio</t>
+  </si>
+  <si>
+    <t>Cultist worship effects</t>
+  </si>
+  <si>
+    <t>Add havoc unit</t>
+  </si>
+  <si>
+    <t>Iterate on Raven to make it a viable unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ravage terror ability </t>
+  </si>
+  <si>
+    <t>Pass on Talos</t>
+  </si>
+  <si>
+    <t>Change cannibalize to ability, iterate on ranged weapon, pathing, check it's damage stats</t>
+  </si>
+  <si>
+    <t>Talos soul harvest ability</t>
+  </si>
+  <si>
+    <t>Starting bike scavange ability rework</t>
+  </si>
+  <si>
+    <t>Scavange ability system</t>
+  </si>
+  <si>
+    <t>Look at rekindled rage global</t>
+  </si>
+  <si>
+    <t>Soul Destruction Design</t>
+  </si>
+  <si>
+    <t>Possibly do this as a zombie ability</t>
+  </si>
+  <si>
+    <t>Add the Incubus Combat squad</t>
+  </si>
+  <si>
+    <t>Design a T3 ranged unit for DE</t>
+  </si>
+  <si>
+    <t>Settle on dark reaper design</t>
+  </si>
+  <si>
+    <t>Get rid of farseer variants</t>
+  </si>
+  <si>
+    <t>Fire dragons alternative effect</t>
+  </si>
+  <si>
+    <t>Merge the eldar embolden abilities</t>
+  </si>
+  <si>
+    <t>Cumulative squad cap for bonesingers</t>
+  </si>
+  <si>
+    <t>Eldar holofields ability</t>
+  </si>
+  <si>
+    <t>Special ability energy system</t>
+  </si>
+  <si>
+    <t>Decide on wraithguard / wraithblade unit</t>
+  </si>
+  <si>
+    <t>Alternative model for anti-infantry vyper</t>
+  </si>
+  <si>
+    <t>Alternative model for eldar subcommander</t>
+  </si>
+  <si>
+    <t>Harlequin kiss ability changed to timed not targeted</t>
+  </si>
+  <si>
+    <t>Revisit warlock sub-commander abilities</t>
+  </si>
+  <si>
+    <t>Fire prism weapon swap ability</t>
+  </si>
+  <si>
+    <t>Change guard assassin to research not addons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decide on Cln Brom </t>
+  </si>
+  <si>
+    <t>Earthshaker ability rework</t>
+  </si>
+  <si>
+    <t>Revert change adding second turret (keep it in files)</t>
+  </si>
+  <si>
+    <t>Turret spawn global for Techmarine OM</t>
+  </si>
+  <si>
+    <t>Turret spawn global for Enginseer</t>
+  </si>
+  <si>
+    <t>Riders Change to updated model</t>
+  </si>
+  <si>
+    <t>Riders leader commissar model</t>
+  </si>
+  <si>
+    <t>Riders new voices</t>
+  </si>
+  <si>
+    <t>Rework hellhound T3 ability</t>
+  </si>
+  <si>
+    <t>Leman Russ side arms lascannon bug fix</t>
+  </si>
+  <si>
+    <t>Rework marauder bomba</t>
+  </si>
+  <si>
+    <t>Bomb ability reworked into the combat and chang these bombs via weapon upgrades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redo marauder bombing run ability for smoke </t>
+  </si>
+  <si>
+    <t>Effects for ogryn abilities</t>
+  </si>
+  <si>
+    <t>Sentinel and scout sentinel stomp animation</t>
+  </si>
+  <si>
+    <t>Artillery spotters model</t>
+  </si>
+  <si>
+    <t>Artillery spotter Icon</t>
+  </si>
+  <si>
+    <t>Artillery spotter voice</t>
+  </si>
+  <si>
+    <t>Artillery spotter ability icons</t>
+  </si>
+  <si>
+    <t>Remove spotter vision ability</t>
+  </si>
+  <si>
+    <t>Reworkand re-add secondary artillery abilty to a mixed use smoke</t>
   </si>
 </sst>
 </file>
@@ -172,7 +521,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,8 +600,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBC0BB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -268,9 +629,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -279,7 +638,16 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -289,86 +657,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -376,7 +795,19 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="256">
+  <dxfs count="147">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFDC7EC3"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -877,6 +1308,18 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
+          <bgColor rgb="FFDC7EC3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
@@ -1369,6 +1812,18 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
+          <bgColor rgb="FFDC7EC3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
@@ -1598,1350 +2053,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFCAE2BC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDC7EC3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF7DBEC1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD3D7BB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD7EDA5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFE20000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD28EF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF84FA9A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF4F4F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF872D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC0F973"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF872D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF4F4F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC0F973"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCAE2BC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF7DBEC1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD3D7BB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD7EDA5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFE20000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD28EF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF84FA9A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF4F4F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF872D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC0F973"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF872D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF4F4F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC0F973"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCAE2BC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDC7EC3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF7DBEC1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD3D7BB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD7EDA5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFE20000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD28EF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF84FA9A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF4F4F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF872D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC0F973"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF872D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF4F4F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC0F973"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCAE2BC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFE20000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF7DBEC1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD3D7BB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD7EDA5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFE20000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD28EF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF84FA9A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF4F4F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF872D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC0F973"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF872D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF4F4F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC0F973"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCAE2BC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDC7EC3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF7DBEC1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD3D7BB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD7EDA5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFE20000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD28EF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF84FA9A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF4F4F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF872D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC0F973"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF872D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF4F4F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC0F973"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFCAE2BC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF7DBEC1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD3D7BB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD7EDA5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFE20000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3453,6 +2564,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFBC0BB"/>
       <color rgb="FFDC7EC3"/>
       <color rgb="FFE20000"/>
       <color rgb="FF9954CC"/>
@@ -3462,7 +2574,6 @@
       <color rgb="FFFFCDF4"/>
       <color rgb="FFD28EF0"/>
       <color rgb="FF84FA9A"/>
-      <color rgb="FFD7EDA5"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3739,56 +2850,995 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE0C65C-144B-49AC-9C67-3120B47D1850}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="14" style="20" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="20" customWidth="1"/>
-    <col min="7" max="7" width="121.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4" hidden="1"/>
+    <col min="1" max="1" width="55.42578125" style="40" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="41" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="42" customWidth="1"/>
+    <col min="4" max="4" width="14" style="42" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="42" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="42" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="40" customWidth="1"/>
+    <col min="8" max="8" width="0" style="44" hidden="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="44" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="38" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F2" s="21"/>
+      <c r="A2" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F3" s="21"/>
+      <c r="A3" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="43"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="43" t="str">
+        <f>HYPERLINK("#'Design'!A6",Design!A6)</f>
+        <v>Balancing Tau</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="43" t="str">
+        <f>HYPERLINK("#'Design'!A10",Design!A10)</f>
+        <v>Armour Resistance Rework</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="43" t="str">
+        <f>HYPERLINK("#'Code'!A3","Code system")</f>
+        <v>Code system</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="43" t="str">
+        <f>HYPERLINK("#'Code'!A4","Souls Abil")</f>
+        <v>Souls Abil</v>
+      </c>
+      <c r="G32" s="40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="43" t="str">
+        <f>HYPERLINK("#'Code'!A5","Scavange Abil")</f>
+        <v>Scavange Abil</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="40" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="43" t="str">
+        <f>HYPERLINK("#'Code'!A6","Energy System")</f>
+        <v>Energy System</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="B49" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="B50" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="B51" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="B52" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" s="40" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="B54" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="42" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4165,56 +4215,191 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6536BA35-512A-45A9-A1C5-27E1FD846304}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="14" style="14" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="121.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4" hidden="1"/>
+    <col min="1" max="1" width="55.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="14" style="10" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="0" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F2" s="15"/>
+      <c r="A2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="11" t="str">
+        <f>HYPERLINK("#'Design'!A2","EBPs/SBPs")</f>
+        <v>EBPs/SBPs</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F3" s="15"/>
+      <c r="A3" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4591,56 +4776,103 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD4FD48-59DA-4679-9E2B-5C148A159A94}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="26" customWidth="1"/>
-    <col min="4" max="4" width="14" style="26" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="26" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="121.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4" hidden="1"/>
+    <col min="1" max="1" width="55.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="14" style="18" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="16" customWidth="1"/>
+    <col min="8" max="8" width="0" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F2" s="27"/>
+      <c r="A2" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F3" s="27"/>
+      <c r="A3" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5017,56 +5249,449 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="14" style="8" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="121.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4" hidden="1"/>
+    <col min="1" max="1" width="55.42578125" style="44" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="49" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="50" customWidth="1"/>
+    <col min="4" max="4" width="14" style="50" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="50" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="50" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="44" customWidth="1"/>
+    <col min="8" max="8" width="0" style="44" hidden="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="44" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="47" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F3" s="9"/>
+      <c r="A2" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="51"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="51" t="str">
+        <f>HYPERLINK("#'Art'!A4","Check Cur Model")</f>
+        <v>Check Cur Model</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5442,57 +6067,808 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64EFB410-336E-427B-AD81-884224B59A7F}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAB2C39-26AB-4D6A-97C6-B18CDA37BA1E}">
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" style="31" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="32" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="33" customWidth="1"/>
-    <col min="4" max="4" width="14" style="33" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="33" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="33" customWidth="1"/>
-    <col min="7" max="7" width="121.85546875" style="31" customWidth="1"/>
-    <col min="8" max="8" width="0" style="31" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="31" hidden="1"/>
+    <col min="1" max="1" width="55.42578125" style="56" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="57" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="58" customWidth="1"/>
+    <col min="4" max="4" width="14" style="58" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="58" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="58" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="56" customWidth="1"/>
+    <col min="8" max="8" width="0" style="56" hidden="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="56" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="54" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F2" s="34"/>
+      <c r="A2" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="59"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F3" s="34"/>
+      <c r="A3" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="59"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="58" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="56" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="58" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="17" id="{5F89D456-C1D7-4584-B39B-0943F95C9FE9}">
+            <xm:f>$B2 = Macro!$A$6</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FFCAE2BC"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="18" id="{894C1261-6556-4A65-945F-31A79C95F1D9}">
+            <xm:f>$B2 = Macro!$A$5</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FFC0F973"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="19" id="{A7E9D8E9-3895-4361-9C09-C81ECD1A9CF1}">
+            <xm:f>$B2 = Macro!$A$4</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor theme="7"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="20" id="{7A01F87B-48A8-4C58-84D6-FB4FD5B06B2A}">
+            <xm:f>$B2 = Macro!$A$2</xm:f>
+            <x14:dxf>
+              <font>
+                <b/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FFFF4F4F"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="21" id="{B3F21F71-8DA2-4067-84E4-F3A6DB364881}">
+            <xm:f>$B2 = Macro!$A$3</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FFFF872D"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="13" id="{E930375C-7A59-4F8E-A437-81F1910A24F4}">
+            <xm:f>$C2 = Macro!$B$5</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FFC0F973"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="14" id="{83B5F26B-61F7-48E3-89F7-E7F9856C48D5}">
+            <xm:f>$C2 = Macro!$B$3</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FFFF872D"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="15" id="{4A13A275-27A6-4A39-93A8-128093A32EFA}">
+            <xm:f>$C2 = Macro!$B$4</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor theme="7"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="16" id="{8D97C3D6-E320-4D63-A85B-77493D234883}">
+            <xm:f>$C2 = Macro!$B$2</xm:f>
+            <x14:dxf>
+              <font>
+                <b/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FFFF4F4F"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="2" id="{53401B61-8C26-4936-AF37-010EFCD3E11A}">
+            <xm:f>$D2 = Macro!$C$4</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FF84FA9A"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="3" id="{CE7476A5-A8B6-4F52-BBAF-408F72BBA18E}">
+            <xm:f>$D2 = Macro!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FFD28EF0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="4" id="{4973F71B-0CD8-4A06-94D1-0E234C5146CE}">
+            <xm:f>$D2 = Macro!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor theme="0" tint="-0.24994659260841701"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{2DED8810-85D1-479E-9B76-B0E30FD5A61B}">
+            <xm:f>$E2 = Macro!$D$10</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FFDC7EC3"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="5" id="{E5D82F8A-CCFD-4820-8690-EEA654512B55}">
+            <xm:f>$E2 = Macro!$D$9</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FFE20000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="6" id="{AA70FDF2-6F6D-4032-9AA4-B72BE8EA3E91}">
+            <xm:f>$E2 = Macro!$D$8</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="7" id="{401B3AE6-14F5-45E8-B567-9E2F2ACFA9A6}">
+            <xm:f>$E2 = Macro!$D$7</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FFD7EDA5"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="8" id="{8FFD208F-7BC3-4F57-9983-67A453E70B12}">
+            <xm:f>$E2 = Macro!$D$6</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FFD3D7BB"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="9" id="{F706DB69-B081-44FF-8284-F40C77F25E4C}">
+            <xm:f>$E2 = Macro!$D$5</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor theme="7" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="10" id="{1758B631-052C-41AE-9E68-1D5729D09491}">
+            <xm:f>$E2 = Macro!$D$3</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="11" id="{C4FB43B3-0892-46BF-A59C-F919F3E09FFB}">
+            <xm:f>$E2 = Macro!$D$4</xm:f>
+            <x14:dxf>
+              <font>
+                <b/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor rgb="FF7DBEC1"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="12" id="{4CDF84FF-5809-4DDA-9C38-C94ED09C6886}">
+            <xm:f>$E2 = Macro!$D$2</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+              </font>
+              <numFmt numFmtId="0" formatCode="General"/>
+              <fill>
+                <patternFill patternType="solid">
+                  <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Use the dropdown to select a vaid priority." promptTitle="Status" prompt="What is the progress on this?" xr:uid="{49DD2C91-129D-4BBD-8108-73F9DDC2818D}">
+          <x14:formula1>
+            <xm:f>Macro!$D$2:$D$1000</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Use the dropdown to select a vaid priority." promptTitle="Assignee" prompt="Who will work on this?" xr:uid="{FE1C7C26-A819-4513-80A6-98F61FA43D59}">
+          <x14:formula1>
+            <xm:f>Macro!$C$2:$C$1000</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Use the dropdown to select a vaid priority." promptTitle="Severity" prompt="How important is this?" xr:uid="{FE95ED34-1CEA-4FD8-BBB5-D3C5C3671D45}">
+          <x14:formula1>
+            <xm:f>Macro!$B$2:$B$1000</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Use the dropdown to select a vaid priority." promptTitle="Priority" prompt="How soon do we want to do this?" xr:uid="{F4AFAFF2-0F7A-4031-92E4-C12B14E4BC14}">
+          <x14:formula1>
+            <xm:f>Macro!$A$2:$A$1000</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Use the dropdown to select a vaid priority." promptTitle="Priority" prompt="How serious is this?" xr:uid="{5554F558-F147-413C-98B5-E5965C60BC9F}">
+          <x14:formula1>
+            <xm:f>Macro!$A$2:$A$1000</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64EFB410-336E-427B-AD81-884224B59A7F}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B1048544" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.42578125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="14" style="26" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="26" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="24" customWidth="1"/>
+    <col min="8" max="8" width="0" style="24" hidden="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="24" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5867,58 +7243,58 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752D83A-575D-48F9-8AB2-691C59C846FF}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1048544" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" style="41" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="42" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="43" customWidth="1"/>
-    <col min="4" max="4" width="14" style="43" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="43" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="43" customWidth="1"/>
-    <col min="7" max="7" width="121.85546875" style="41" customWidth="1"/>
-    <col min="8" max="8" width="0" style="41" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="41" hidden="1"/>
+    <col min="1" max="1" width="55.42578125" style="32" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="33" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="14" style="34" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="34" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="34" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="32" customWidth="1"/>
+    <col min="8" max="8" width="0" style="32" hidden="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="32" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F2" s="44"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F3" s="44"/>
+      <c r="F3" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6293,12 +7669,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CBD162-1EFD-4ED3-B005-8CE300437CD8}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6310,16 +7686,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I1" t="s">
@@ -6339,7 +7715,7 @@
       <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="6" t="str">
+      <c r="I2" s="2" t="str">
         <f>HYPERLINK("#'Code'!A1",Code!A1)</f>
         <v>Task</v>
       </c>
@@ -6378,6 +7754,9 @@
       </c>
       <c r="B5" t="s">
         <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
       </c>
       <c r="D5" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
[PLANNING] Updated planning notes to show show whats been done for this week
</commit_message>
<xml_diff>
--- a/Development/Planning/TaskPlanning.xlsx
+++ b/Development/Planning/TaskPlanning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files (x86)\Steam\steamapps\common\Dawn of War Soulstorm\TFE\Development\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Dawn of War Soulstorm\TFE\Development\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB7AE1F-C858-4868-8BC4-5DB828779BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27EDD09-2FD3-4391-A917-6549B4F794BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="9" r:id="rId1"/>
@@ -699,9 +699,6 @@
     <t>Rework apothecary combat stims ability</t>
   </si>
   <si>
-    <t>Rework apothecary to have bolter</t>
-  </si>
-  <si>
     <t>SM Shotgun blast rewritten as a high explosive round</t>
   </si>
   <si>
@@ -742,6 +739,9 @@
   </si>
   <si>
     <t>Rework drone harbinger so that its drones auto follow it and auto attack</t>
+  </si>
+  <si>
+    <t>Rework apothecary to have bolt pistol</t>
   </si>
 </sst>
 </file>
@@ -752,7 +752,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -760,7 +760,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -768,7 +768,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1060,8 +1060,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="ارتباط تشعبي" xfId="1" builtinId="8"/>
-    <cellStyle name="عادي" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="147">
     <dxf>
@@ -3121,26 +3121,26 @@
   <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.375" style="24" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="25.375" style="26" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="26" customWidth="1"/>
     <col min="4" max="4" width="14" style="26" customWidth="1"/>
-    <col min="5" max="5" width="22.875" style="26" customWidth="1"/>
-    <col min="6" max="6" width="14.75" style="26" customWidth="1"/>
-    <col min="7" max="7" width="121.875" style="24" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="26" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="24" customWidth="1"/>
     <col min="8" max="8" width="0" style="28" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="28" hidden="1"/>
+    <col min="9" max="16384" width="9.140625" style="28" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>34</v>
       </c>
@@ -3177,11 +3177,11 @@
         <v>8</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F2" s="27"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>33</v>
       </c>
@@ -3195,11 +3195,11 @@
         <v>8</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F3" s="27"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>36</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>37</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>40</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>41</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>42</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>Balancing Tau</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>43</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>44</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>46</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>Armour Resistance Rework</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>47</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>48</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>49</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>53</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>54</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>55</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>56</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>57</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>59</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>60</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>82</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>83</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>84</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>85</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>86</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
         <v>91</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>Code system</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>97</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>101</v>
       </c>
@@ -3662,10 +3662,10 @@
         <v>8</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
         <v>102</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>103</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>104</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
         <v>107</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>Scavange Abil</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>109</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>110</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>112</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>113</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>114</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>115</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>117</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>118</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>119</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>Energy System</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>121</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
         <v>124</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
         <v>125</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="24" t="s">
         <v>126</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
         <v>127</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
         <v>128</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
         <v>129</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
         <v>130</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
         <v>136</v>
       </c>
@@ -4057,7 +4057,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
         <v>138</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
         <v>147</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
         <v>148</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
         <v>149</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
         <v>150</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
         <v>151</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
         <v>157</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
         <v>158</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
         <v>161</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
         <v>162</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="24" t="s">
         <v>164</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
         <v>165</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
         <v>169</v>
       </c>
@@ -4287,7 +4287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
         <v>170</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
         <v>171</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="24" t="s">
         <v>172</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>Energy System</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="24" t="s">
         <v>173</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="24" t="s">
         <v>174</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="24" t="s">
         <v>177</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
         <v>180</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>New Model</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="24" t="s">
         <v>185</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
         <v>187</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
         <v>191</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
         <v>192</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
         <v>193</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="24" t="s">
         <v>194</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="s">
         <v>195</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="24" t="s">
         <v>196</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="24" t="s">
         <v>200</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
         <v>201</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="24" t="s">
         <v>207</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
         <v>208</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="24" t="s">
         <v>210</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>Holy Piercing</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
         <v>211</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="24" t="s">
         <v>213</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="24" t="s">
         <v>215</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="24" t="s">
         <v>217</v>
       </c>
@@ -4722,9 +4722,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B89" s="25" t="s">
         <v>12</v>
@@ -4739,9 +4739,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B90" s="25" t="s">
         <v>11</v>
@@ -4756,9 +4756,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B91" s="25" t="s">
         <v>11</v>
@@ -4773,9 +4773,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B92" s="25" t="s">
         <v>11</v>
@@ -4790,9 +4790,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B93" s="25" t="s">
         <v>12</v>
@@ -4807,9 +4807,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B94" s="25" t="s">
         <v>12</v>
@@ -4828,9 +4828,9 @@
         <v>Energy System</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B95" s="25" t="s">
         <v>13</v>
@@ -4845,9 +4845,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B96" s="25" t="s">
         <v>11</v>
@@ -4862,9 +4862,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B97" s="25" t="s">
         <v>11</v>
@@ -5263,20 +5263,20 @@
       <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.375" style="56" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="57" customWidth="1"/>
-    <col min="3" max="3" width="25.375" style="58" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" style="56" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="57" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="58" customWidth="1"/>
     <col min="4" max="4" width="14" style="58" customWidth="1"/>
-    <col min="5" max="5" width="22.875" style="58" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="58" customWidth="1"/>
-    <col min="7" max="7" width="121.875" style="56" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="58" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="58" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="56" customWidth="1"/>
     <col min="8" max="8" width="0" style="28" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="28" hidden="1"/>
+    <col min="9" max="16384" width="9.140625" style="28" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="55" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>35</v>
       </c>
@@ -5320,7 +5320,7 @@
         <v>EBPs/SBPs</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>90</v>
       </c>
@@ -5338,7 +5338,7 @@
       </c>
       <c r="F3" s="59"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>106</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
         <v>108</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
         <v>120</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
         <v>131</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
         <v>132</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
         <v>140</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
         <v>183</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
         <v>203</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
         <v>205</v>
       </c>
@@ -5494,9 +5494,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B13" s="57" t="s">
         <v>11</v>
@@ -5511,9 +5511,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B14" s="57" t="s">
         <v>11</v>
@@ -5528,12 +5528,12 @@
         <v>22</v>
       </c>
       <c r="G14" s="56" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="56" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B15" s="57" t="s">
         <v>12</v>
@@ -5932,20 +5932,20 @@
       <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="25.375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="10" customWidth="1"/>
     <col min="4" max="4" width="14" style="10" customWidth="1"/>
-    <col min="5" max="5" width="22.875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="121.875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="8" customWidth="1"/>
     <col min="8" max="8" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="3" hidden="1"/>
+    <col min="9" max="16384" width="9.140625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>99</v>
       </c>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>135</v>
       </c>
@@ -6004,7 +6004,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>145</v>
       </c>
@@ -6402,23 +6402,23 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F44" sqref="F44"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.375" style="28" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="33" customWidth="1"/>
-    <col min="3" max="3" width="25.375" style="34" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="33" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="34" customWidth="1"/>
     <col min="4" max="4" width="14" style="34" customWidth="1"/>
-    <col min="5" max="5" width="22.875" style="34" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="34" customWidth="1"/>
-    <col min="7" max="7" width="121.875" style="28" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="34" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="34" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="28" customWidth="1"/>
     <col min="8" max="8" width="0" style="28" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="28" hidden="1"/>
+    <col min="9" max="16384" width="9.140625" style="28" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>50</v>
       </c>
@@ -6459,7 +6459,7 @@
       </c>
       <c r="F2" s="35"/>
     </row>
-    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
@@ -6480,7 +6480,7 @@
         <v>Check Cur Model</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>52</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>87</v>
       </c>
@@ -6514,7 +6514,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>88</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>89</v>
       </c>
@@ -6548,7 +6548,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>93</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>92</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>94</v>
       </c>
@@ -6599,7 +6599,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
         <v>95</v>
       </c>
@@ -6619,7 +6619,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
         <v>98</v>
       </c>
@@ -6636,7 +6636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
         <v>100</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
         <v>116</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>122</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
         <v>123</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
         <v>133</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>134</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>137</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
         <v>141</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>142</v>
       </c>
@@ -6789,7 +6789,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>143</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
         <v>144</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>146</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
         <v>152</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
         <v>153</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>154</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
         <v>155</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
         <v>156</v>
       </c>
@@ -6925,7 +6925,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
         <v>160</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>163</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>167</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
         <v>168</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
         <v>176</v>
       </c>
@@ -7010,7 +7010,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
         <v>179</v>
       </c>
@@ -7027,7 +7027,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>181</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>182</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
         <v>186</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
         <v>189</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
         <v>190</v>
       </c>
@@ -7112,7 +7112,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>197</v>
       </c>
@@ -7129,7 +7129,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
         <v>206</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>209</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
         <v>212</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
         <v>214</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>216</v>
       </c>
@@ -7214,9 +7214,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="B47" s="33" t="s">
         <v>13</v>
@@ -7228,12 +7228,12 @@
         <v>8</v>
       </c>
       <c r="E47" s="34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B48" s="33" t="s">
         <v>11</v>
@@ -7632,20 +7632,20 @@
       <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.375" style="40" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="41" customWidth="1"/>
-    <col min="3" max="3" width="25.375" style="42" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" style="40" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="41" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="42" customWidth="1"/>
     <col min="4" max="4" width="14" style="42" customWidth="1"/>
-    <col min="5" max="5" width="22.875" style="42" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="42" customWidth="1"/>
-    <col min="7" max="7" width="121.875" style="40" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="42" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="42" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="40" customWidth="1"/>
     <col min="8" max="8" width="0" style="40" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="40" hidden="1"/>
+    <col min="9" max="16384" width="9.140625" style="40" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="39" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -7668,7 +7668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>61</v>
       </c>
@@ -7686,7 +7686,7 @@
       </c>
       <c r="F2" s="43"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>74</v>
       </c>
@@ -7704,7 +7704,7 @@
       </c>
       <c r="F3" s="43"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>75</v>
       </c>
@@ -7721,7 +7721,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
         <v>76</v>
       </c>
@@ -7741,7 +7741,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
         <v>77</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
         <v>78</v>
       </c>
@@ -7775,7 +7775,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
         <v>62</v>
       </c>
@@ -7792,7 +7792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
         <v>63</v>
       </c>
@@ -7809,7 +7809,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
         <v>64</v>
       </c>
@@ -7826,7 +7826,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
         <v>65</v>
       </c>
@@ -7843,7 +7843,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>68</v>
       </c>
@@ -7860,7 +7860,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
         <v>67</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
         <v>69</v>
       </c>
@@ -7894,7 +7894,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
         <v>70</v>
       </c>
@@ -7911,7 +7911,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
         <v>71</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
         <v>72</v>
       </c>
@@ -7945,7 +7945,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
         <v>73</v>
       </c>
@@ -7965,7 +7965,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
         <v>79</v>
       </c>
@@ -7982,7 +7982,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
         <v>80</v>
       </c>
@@ -8383,20 +8383,20 @@
       <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.375" style="48" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="49" customWidth="1"/>
-    <col min="3" max="3" width="25.375" style="50" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" style="48" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="49" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="50" customWidth="1"/>
     <col min="4" max="4" width="14" style="50" customWidth="1"/>
-    <col min="5" max="5" width="22.875" style="50" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="50" customWidth="1"/>
-    <col min="7" max="7" width="121.875" style="48" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="50" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="50" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="48" customWidth="1"/>
     <col min="8" max="8" width="0" style="48" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="48" hidden="1"/>
+    <col min="9" max="16384" width="9.140625" style="48" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="47" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -8419,7 +8419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>198</v>
       </c>
@@ -8437,7 +8437,7 @@
       </c>
       <c r="F2" s="51"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3" s="51"/>
     </row>
   </sheetData>
@@ -8824,20 +8824,20 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="17" customWidth="1"/>
-    <col min="3" max="3" width="25.375" style="18" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="18" customWidth="1"/>
     <col min="4" max="4" width="14" style="18" customWidth="1"/>
-    <col min="5" max="5" width="22.875" style="18" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="121.875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="121.85546875" style="16" customWidth="1"/>
     <col min="8" max="8" width="0" style="16" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="16" hidden="1"/>
+    <col min="9" max="16384" width="9.140625" style="16" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -8860,10 +8860,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3" s="19"/>
     </row>
   </sheetData>
@@ -9247,15 +9247,15 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -9272,7 +9272,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -9290,7 +9290,7 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -9304,7 +9304,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -9318,7 +9318,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -9332,7 +9332,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -9340,22 +9340,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
[PLANNING] Move notes from Discord to excel
</commit_message>
<xml_diff>
--- a/Development/Planning/TaskPlanning.xlsx
+++ b/Development/Planning/TaskPlanning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Dawn of War Soulstorm\TFE\Development\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27EDD09-2FD3-4391-A917-6549B4F794BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21651B69-FA08-4D49-82D8-E64C6B0D4E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="9" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="298">
   <si>
     <t>Task</t>
   </si>
@@ -742,6 +742,201 @@
   </si>
   <si>
     <t>Rework apothecary to have bolt pistol</t>
+  </si>
+  <si>
+    <t>List of units excluded from cover</t>
+  </si>
+  <si>
+    <t>True random race scar</t>
+  </si>
+  <si>
+    <t>This is currently broken</t>
+  </si>
+  <si>
+    <t>Refactor to import scar files as variables instead of making them global</t>
+  </si>
+  <si>
+    <t>Look into Titanium wars level up UI</t>
+  </si>
+  <si>
+    <t>Consistency between the different healing / draining effects such as heal over time and instant heal</t>
+  </si>
+  <si>
+    <t>Look into "ScatterFromSquad</t>
+  </si>
+  <si>
+    <t>Units with dozer blades able to destroy mines by running them over</t>
+  </si>
+  <si>
+    <t>Possibly implement Die Last Leaders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduce overlap between reclemator and tomb spyder </t>
+  </si>
+  <si>
+    <t>Possibly tomb spyder melee range res orb instead of harvest?</t>
+  </si>
+  <si>
+    <t>Look into every faction to test if they have the tier scaling for requisition</t>
+  </si>
+  <si>
+    <t>Cosmetic music scar, should we keep it? If so finish it</t>
+  </si>
+  <si>
+    <t>Don't forget to add I.H and Nids here</t>
+  </si>
+  <si>
+    <t>To find exact locations of where entities die, use "spawn_on_death". Perhaps with a unique entity for each squad BP?</t>
+  </si>
+  <si>
+    <t>Take another look at Ork post T4 upgrades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add a generic class manager to run Updates </t>
+  </si>
+  <si>
+    <t>Use a table</t>
+  </si>
+  <si>
+    <t>BR Move Starting location to be slightly more forward</t>
+  </si>
+  <si>
+    <t>Rework mind war scaling</t>
+  </si>
+  <si>
+    <t>Torture amp causes units who die around it to generate souls</t>
+  </si>
+  <si>
+    <t>Any units DE kills gives a small number of souls to the killer</t>
+  </si>
+  <si>
+    <t>Remove passive soul gen after 30 souls after this?</t>
+  </si>
+  <si>
+    <t>Experiment with transferring units to your allies</t>
+  </si>
+  <si>
+    <t>Most interestingly rhinos</t>
+  </si>
+  <si>
+    <t>Remove initial delay time from global abilities</t>
+  </si>
+  <si>
+    <t>Take another look at Tau population system</t>
+  </si>
+  <si>
+    <t>Tau give Snapshot a wind up time</t>
+  </si>
+  <si>
+    <t>TC Snap shot animation</t>
+  </si>
+  <si>
+    <t>Stop Stikkbombas smoke effect not stacking</t>
+  </si>
+  <si>
+    <t>Move combat drones to Tier 1 buildable from barracks</t>
+  </si>
+  <si>
+    <t>Move pathfinder ability to T1 and check if it needs rebalances</t>
+  </si>
+  <si>
+    <t>Look at special attacks and make sure that all melee units who need it have it</t>
+  </si>
+  <si>
+    <t>Animations for special attacks on squads like raptors</t>
+  </si>
+  <si>
+    <t>"Party Mode" for larger FFA games</t>
+  </si>
+  <si>
+    <t>Brainstorm alternative winconditions like capture the hill</t>
+  </si>
+  <si>
+    <t>Capture the flag? King of the hill?</t>
+  </si>
+  <si>
+    <t>Tau crisis suits withwider variety of weapons? Double chiaingun?</t>
+  </si>
+  <si>
+    <t>Rites of exorcism deals more damage to Daemons</t>
+  </si>
+  <si>
+    <t>Grenade abilities should not chase squads when selecting the squad</t>
+  </si>
+  <si>
+    <t>"Regicide" achievement, first person to kill a commander</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Killing LPs is currently counting as killing gens? </t>
+  </si>
+  <si>
+    <t>Achievement ssytesm</t>
+  </si>
+  <si>
+    <t>Take another look at drop pod global for SM and give it fun bonuses</t>
+  </si>
+  <si>
+    <t>Deploy smoke on land in star around the drop pod, and heal nearby units</t>
+  </si>
+  <si>
+    <t>We need some way for of understanding combat in relation to entities (entity killing squad, or squad killing entity)</t>
+  </si>
+  <si>
+    <t>World_GetSpawnablePosition</t>
+  </si>
+  <si>
+    <t>Rework Tyranids auto builder to be more effective</t>
+  </si>
+  <si>
+    <t>Take a look at penalising tyranids when they lose a structure</t>
+  </si>
+  <si>
+    <t>Importantly look over the Dev_SetupAutoConstructors  in GlobalAbilities_Core as it might be depreciated. If it isn't depreciated, it needs to be redone as it's currently creating an auto builder just for player 1?</t>
+  </si>
+  <si>
+    <t>I need to really look into this auto builder carefully</t>
+  </si>
+  <si>
+    <t>Use Player_CanSeePosition to check if something is in fog of war, thus allowing you to stop globals being casted outside fow</t>
+  </si>
+  <si>
+    <t>Cryptek abilities for recycling bodies for scarab stuff?</t>
+  </si>
+  <si>
+    <t>Check if relocate can be used on squads?</t>
+  </si>
+  <si>
+    <t>Alternative TP for necron</t>
+  </si>
+  <si>
+    <t>Remove cost for Hive tyrant weapon swap ability and make the hive tyrant pay with HP</t>
+  </si>
+  <si>
+    <t>Wings for Hive tyrant given on T2, not an addon</t>
+  </si>
+  <si>
+    <t>Improve pathing around mountains, check middle path on the opened up mountains, possibly adjust crit positions</t>
+  </si>
+  <si>
+    <t>New Map: Long bridge</t>
+  </si>
+  <si>
+    <t>New Map: Poison Cover</t>
+  </si>
+  <si>
+    <t>New Map: Asymetrical Map</t>
+  </si>
+  <si>
+    <t>New Map: Height Cover Emphasis</t>
+  </si>
+  <si>
+    <t>Rocky Valley? No Man's Land?</t>
+  </si>
+  <si>
+    <t>New Map: Open Map that does not guide the player</t>
+  </si>
+  <si>
+    <t>This is pretty much EG though….</t>
   </si>
 </sst>
 </file>
@@ -3118,13 +3313,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE0C65C-144B-49AC-9C67-3120B47D1850}">
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A100" sqref="A100"/>
+      <selection pane="bottomRight" activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4862,7 +5057,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="24" t="s">
         <v>230</v>
       </c>
@@ -4876,6 +5071,379 @@
         <v>21</v>
       </c>
       <c r="E97" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="B98" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C98" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E98" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G98" s="24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="B99" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C99" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D99" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E99" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B100" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D100" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="B101" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D101" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E101" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="B102" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C102" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D102" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E102" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="B103" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C103" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D103" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E103" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F103" s="27" t="str">
+        <f>HYPERLINK("#'Art'!A50","Animation")</f>
+        <v>Animation</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="B104" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C104" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D104" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="B105" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C105" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D105" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="B106" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C106" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D106" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E106" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="B107" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C107" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D107" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E107" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="B108" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C108" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D108" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E108" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="B109" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C109" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D109" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E109" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G109" s="24" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="B110" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C110" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D110" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E110" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="B111" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C111" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D111" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="B112" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C112" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D112" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E112" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="B113" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C113" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D113" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E113" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="B114" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C114" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D114" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E114" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G114" s="24" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="B115" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C115" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E115" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="B116" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C116" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D116" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E116" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="B117" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C117" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D117" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E117" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G117" s="24" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="B118" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D118" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E118" s="26" t="s">
         <v>22</v>
       </c>
     </row>
@@ -5215,7 +5783,7 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="860" yWindow="605" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Use the dropdown to select a vaid priority." promptTitle="Priority" prompt="How serious is this?" xr:uid="{7800D482-4501-4EA0-9B5D-A800AB0A8E90}">
           <x14:formula1>
             <xm:f>Macro!$A$2:$A$1000</xm:f>
@@ -5254,13 +5822,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6536BA35-512A-45A9-A1C5-27E1FD846304}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5545,6 +6113,333 @@
         <v>7</v>
       </c>
       <c r="E15" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="56" t="s">
+        <v>233</v>
+      </c>
+      <c r="B16" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="56" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>236</v>
+      </c>
+      <c r="B18" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="56" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="56" t="s">
+        <v>241</v>
+      </c>
+      <c r="B22" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="56" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="B24" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="s">
+        <v>249</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="56" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="B26" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="B27" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="56" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="56" t="s">
+        <v>256</v>
+      </c>
+      <c r="B28" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="56" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="56" t="s">
+        <v>278</v>
+      </c>
+      <c r="B29" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="B30" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="56" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="56" t="s">
+        <v>282</v>
+      </c>
+      <c r="B31" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="56" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="56" t="s">
+        <v>284</v>
+      </c>
+      <c r="B32" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="56" t="s">
+        <v>288</v>
+      </c>
+      <c r="B33" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="58" t="s">
         <v>22</v>
       </c>
     </row>
@@ -6396,13 +7291,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7245,6 +8140,57 @@
         <v>7</v>
       </c>
       <c r="E48" s="34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="B49" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="B50" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="B51" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="34" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7623,13 +8569,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAB2C39-26AB-4D6A-97C6-B18CDA37BA1E}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7910,6 +8856,9 @@
       <c r="E15" s="42" t="s">
         <v>28</v>
       </c>
+      <c r="G15" s="40" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
@@ -7997,6 +8946,114 @@
       </c>
       <c r="E20" s="42" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="40" t="s">
+        <v>291</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="40" t="s">
+        <v>292</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="40" t="s">
+        <v>294</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="40" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="40" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -8374,13 +9431,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64EFB410-336E-427B-AD81-884224B59A7F}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8437,8 +9494,43 @@
       </c>
       <c r="F2" s="51"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>22</v>
+      </c>
       <c r="F3" s="51"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="48" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="48" t="s">
+        <v>275</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8818,10 +9910,10 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1048544" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>